<commit_message>
All that's left is to do the readme properly and you're done.
</commit_message>
<xml_diff>
--- a/PrimeIntellect_Test_GPU_Models.xlsx
+++ b/PrimeIntellect_Test_GPU_Models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sequi\Documents\Projets\prime-intellect-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5C84A9-D83D-4223-9C98-BBA8DE9ED36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7C4FB8-96DD-4A3E-B221-5C79E7470B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>Nemotron</t>
   </si>
@@ -110,12 +110,12 @@
     <t>Models are trained on yahma/alpaca-cleaned dataset.</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>Note</t>
   </si>
   <si>
-    <t>Accuracy is an average of 5 test runs of the cais/mmlu dataset on H100.</t>
-  </si>
-  <si>
     <t>VRAM</t>
   </si>
   <si>
@@ -123,6 +123,21 @@
   </si>
   <si>
     <t>RunPod</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>Disk Size</t>
+  </si>
+  <si>
+    <t>I wish Accuracy is an average of 5 test runs of the cais/mmlu dataset on H100.</t>
+  </si>
+  <si>
+    <t>Actually Accuracy is MMLU score on based pre-trained model.</t>
   </si>
 </sst>
 </file>
@@ -201,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -551,28 +566,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -582,8 +575,71 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -598,63 +654,8 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -664,96 +665,86 @@
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="medium">
@@ -765,12 +756,29 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -778,12 +786,29 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -791,9 +816,11 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -804,22 +831,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -834,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -929,220 +941,223 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1484,84 +1499,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E2:X21"/>
+  <dimension ref="E2:AA23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="2.88671875" style="1" customWidth="1"/>
     <col min="3" max="4" width="0.33203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="11.109375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="15.21875" style="1" customWidth="1"/>
-    <col min="9" max="24" width="9.33203125" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="18.33203125" style="1"/>
+    <col min="5" max="5" width="8.77734375" style="1" customWidth="1"/>
+    <col min="6" max="8" width="7.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.21875" style="1" customWidth="1"/>
+    <col min="12" max="27" width="9.21875" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="18.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="5:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I3" s="59" t="s">
+    <row r="2" spans="5:27" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="5:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="65" t="s">
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
-      <c r="S3" s="66"/>
-      <c r="T3" s="66"/>
-      <c r="U3" s="66"/>
-      <c r="V3" s="66"/>
-      <c r="W3" s="66"/>
-      <c r="X3" s="67"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="48"/>
+      <c r="AA3" s="49"/>
     </row>
-    <row r="4" spans="5:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="5:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="56" t="s">
+      <c r="L4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="53" t="s">
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="50" t="s">
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="52"/>
-      <c r="U4" s="62" t="s">
+      <c r="U4" s="33"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="63"/>
-      <c r="W4" s="63"/>
-      <c r="X4" s="64"/>
+      <c r="Y4" s="45"/>
+      <c r="Z4" s="45"/>
+      <c r="AA4" s="46"/>
     </row>
-    <row r="5" spans="5:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="5:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" s="6" t="s">
         <v>16</v>
       </c>
@@ -1569,438 +1596,634 @@
         <v>16</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="L5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="M5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="N5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="O5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="P5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="Q5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="R5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="15" t="s">
+      <c r="S5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="Q5" s="16" t="s">
+      <c r="T5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="R5" s="17" t="s">
+      <c r="U5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="S5" s="17" t="s">
+      <c r="V5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="T5" s="18" t="s">
+      <c r="W5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="U5" s="19" t="s">
+      <c r="X5" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="V5" s="20" t="s">
+      <c r="Y5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="W5" s="20" t="s">
+      <c r="Z5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="X5" s="21" t="s">
+      <c r="AA5" s="21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:27" x14ac:dyDescent="0.3">
       <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="2">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2">
+        <v>50</v>
+      </c>
+      <c r="H6" s="2">
+        <v>150</v>
+      </c>
+      <c r="I6" s="2">
         <v>80</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="2">
-        <v>1.66</v>
-      </c>
-      <c r="I6" s="88"/>
-      <c r="J6" s="96"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="22">
-        <f>I6*(H6/3600)</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="82"/>
-      <c r="N6" s="97"/>
-      <c r="O6" s="85"/>
-      <c r="P6" s="23">
-        <f>M6*(H6/3600)</f>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="75"/>
-      <c r="R6" s="98"/>
-      <c r="S6" s="78"/>
-      <c r="T6" s="24">
-        <f>Q6*(H6/3600)</f>
-        <v>0</v>
-      </c>
-      <c r="U6" s="68"/>
-      <c r="V6" s="99"/>
-      <c r="W6" s="71"/>
-      <c r="X6" s="25">
-        <f>U6*(H6/3600)</f>
-        <v>0</v>
+      <c r="K6" s="2">
+        <v>1.63</v>
+      </c>
+      <c r="L6" s="68">
+        <v>137</v>
+      </c>
+      <c r="M6" s="85">
+        <v>20.658999999999999</v>
+      </c>
+      <c r="N6" s="71">
+        <v>63.8</v>
+      </c>
+      <c r="O6" s="22">
+        <f>L6*(K6/3600)</f>
+        <v>6.2030555555555554E-2</v>
+      </c>
+      <c r="P6" s="62">
+        <v>186</v>
+      </c>
+      <c r="Q6" s="82">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="R6" s="65">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="S6" s="23">
+        <f>P6*(K6/3600)</f>
+        <v>8.4216666666666662E-2</v>
+      </c>
+      <c r="T6" s="56">
+        <v>201</v>
+      </c>
+      <c r="U6" s="74">
+        <v>1.2410000000000001</v>
+      </c>
+      <c r="V6" s="59">
+        <v>65</v>
+      </c>
+      <c r="W6" s="24">
+        <f>T6*(K6/3600)</f>
+        <v>9.100833333333333E-2</v>
+      </c>
+      <c r="X6" s="50">
+        <v>227</v>
+      </c>
+      <c r="Y6" s="78">
+        <v>2.387</v>
+      </c>
+      <c r="Z6" s="53">
+        <v>64</v>
+      </c>
+      <c r="AA6" s="25">
+        <f>X6*(K6/3600)</f>
+        <v>0.10278055555555556</v>
       </c>
     </row>
-    <row r="7" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:27" x14ac:dyDescent="0.3">
       <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="3">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3">
+        <v>40</v>
+      </c>
+      <c r="H7" s="3">
+        <v>120</v>
+      </c>
+      <c r="I7" s="3">
         <v>80</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="3">
-        <v>0.89</v>
-      </c>
-      <c r="I7" s="89"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="92"/>
-      <c r="L7" s="7">
-        <f>I7*(H7/3600)</f>
-        <v>0</v>
-      </c>
-      <c r="M7" s="83"/>
-      <c r="N7" s="95"/>
-      <c r="O7" s="86"/>
-      <c r="P7" s="8">
-        <f>M7*(H7/3600)</f>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="81"/>
-      <c r="S7" s="79"/>
-      <c r="T7" s="9">
-        <f>Q7*(H7/3600)</f>
-        <v>0</v>
-      </c>
-      <c r="U7" s="69"/>
-      <c r="V7" s="74"/>
-      <c r="W7" s="72"/>
-      <c r="X7" s="26">
-        <f>U7*(H7/3600)</f>
-        <v>0</v>
+      <c r="K7" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="L7" s="69">
+        <v>152</v>
+      </c>
+      <c r="M7" s="86"/>
+      <c r="N7" s="72"/>
+      <c r="O7" s="7">
+        <f>L7*(K7/3600)</f>
+        <v>3.7155555555555553E-2</v>
+      </c>
+      <c r="P7" s="63">
+        <v>246</v>
+      </c>
+      <c r="Q7" s="83"/>
+      <c r="R7" s="66"/>
+      <c r="S7" s="8">
+        <f>P7*(K7/3600)</f>
+        <v>6.013333333333333E-2</v>
+      </c>
+      <c r="T7" s="57">
+        <v>254</v>
+      </c>
+      <c r="U7" s="75"/>
+      <c r="V7" s="60"/>
+      <c r="W7" s="9">
+        <f>T7*(K7/3600)</f>
+        <v>6.2088888888888888E-2</v>
+      </c>
+      <c r="X7" s="51">
+        <v>273</v>
+      </c>
+      <c r="Y7" s="79"/>
+      <c r="Z7" s="54"/>
+      <c r="AA7" s="26">
+        <f>X7*(K7/3600)</f>
+        <v>6.6733333333333325E-2</v>
       </c>
     </row>
-    <row r="8" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:27" x14ac:dyDescent="0.3">
       <c r="E8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="3">
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>30</v>
+      </c>
+      <c r="H8" s="3">
+        <v>100</v>
+      </c>
+      <c r="I8" s="3">
         <v>24</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="3">
-        <v>0.49</v>
-      </c>
-      <c r="I8" s="89"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="7">
-        <f t="shared" ref="L8:L12" si="0">I8*(H8/3600)</f>
-        <v>0</v>
-      </c>
-      <c r="M8" s="83"/>
-      <c r="N8" s="95"/>
-      <c r="O8" s="86"/>
-      <c r="P8" s="8">
-        <f t="shared" ref="P8:P12" si="1">M8*(H8/3600)</f>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="81"/>
-      <c r="S8" s="79"/>
-      <c r="T8" s="9">
-        <f t="shared" ref="T8:T12" si="2">Q8*(H8/3600)</f>
-        <v>0</v>
-      </c>
-      <c r="U8" s="69"/>
-      <c r="V8" s="74"/>
-      <c r="W8" s="72"/>
-      <c r="X8" s="26">
-        <f t="shared" ref="X8:X12" si="3">U8*(H8/3600)</f>
-        <v>0</v>
+      <c r="K8" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="L8" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="86"/>
+      <c r="N8" s="72"/>
+      <c r="O8" s="7" t="e">
+        <f t="shared" ref="O8:O12" si="0">L8*(K8/3600)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P8" s="63">
+        <v>127</v>
+      </c>
+      <c r="Q8" s="83"/>
+      <c r="R8" s="66"/>
+      <c r="S8" s="88">
+        <f>P8*(K8/3600)</f>
+        <v>1.6580555555555557E-2</v>
+      </c>
+      <c r="T8" s="57">
+        <v>169</v>
+      </c>
+      <c r="U8" s="75"/>
+      <c r="V8" s="60"/>
+      <c r="W8" s="9">
+        <f t="shared" ref="W8:W12" si="1">T8*(K8/3600)</f>
+        <v>2.206388888888889E-2</v>
+      </c>
+      <c r="X8" s="51">
+        <v>196</v>
+      </c>
+      <c r="Y8" s="79"/>
+      <c r="Z8" s="54"/>
+      <c r="AA8" s="26">
+        <f t="shared" ref="AA8:AA12" si="2">X8*(K8/3600)</f>
+        <v>2.5588888888888887E-2</v>
       </c>
     </row>
-    <row r="9" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:27" x14ac:dyDescent="0.3">
       <c r="E9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="3">
+        <v>8</v>
+      </c>
+      <c r="G9" s="3">
+        <v>30</v>
+      </c>
+      <c r="H9" s="3">
+        <v>100</v>
+      </c>
+      <c r="I9" s="3">
         <v>48</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="3">
-        <v>0.51</v>
-      </c>
-      <c r="I9" s="89"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="92"/>
-      <c r="L9" s="7">
+      <c r="K9" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="L9" s="69">
+        <v>232</v>
+      </c>
+      <c r="M9" s="86"/>
+      <c r="N9" s="72"/>
+      <c r="O9" s="89">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="83"/>
-      <c r="N9" s="95"/>
-      <c r="O9" s="86"/>
-      <c r="P9" s="8">
+        <v>3.028888888888889E-2</v>
+      </c>
+      <c r="P9" s="63">
+        <v>240</v>
+      </c>
+      <c r="Q9" s="83"/>
+      <c r="R9" s="66"/>
+      <c r="S9" s="8">
+        <f t="shared" ref="S9:S12" si="3">P9*(K9/3600)</f>
+        <v>3.1333333333333331E-2</v>
+      </c>
+      <c r="T9" s="57">
+        <v>240</v>
+      </c>
+      <c r="U9" s="75"/>
+      <c r="V9" s="60"/>
+      <c r="W9" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="76"/>
-      <c r="R9" s="81"/>
-      <c r="S9" s="79"/>
-      <c r="T9" s="9">
+        <v>3.1333333333333331E-2</v>
+      </c>
+      <c r="X9" s="51">
+        <v>314</v>
+      </c>
+      <c r="Y9" s="79"/>
+      <c r="Z9" s="54"/>
+      <c r="AA9" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U9" s="69"/>
-      <c r="V9" s="74"/>
-      <c r="W9" s="72"/>
-      <c r="X9" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.0994444444444444E-2</v>
       </c>
     </row>
-    <row r="10" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:27" x14ac:dyDescent="0.3">
       <c r="E10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="3">
+        <v>9</v>
+      </c>
+      <c r="G10" s="3">
+        <v>50</v>
+      </c>
+      <c r="H10" s="3">
+        <v>100</v>
+      </c>
+      <c r="I10" s="3">
         <v>48</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="3">
+      <c r="K10" s="3">
         <v>0.36</v>
       </c>
-      <c r="I10" s="89"/>
-      <c r="J10" s="94"/>
-      <c r="K10" s="92"/>
-      <c r="L10" s="7">
+      <c r="L10" s="69">
+        <v>217</v>
+      </c>
+      <c r="M10" s="86"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M10" s="83"/>
-      <c r="N10" s="95"/>
-      <c r="O10" s="86"/>
-      <c r="P10" s="8">
+        <v>2.1699999999999997E-2</v>
+      </c>
+      <c r="P10" s="63">
+        <v>180</v>
+      </c>
+      <c r="Q10" s="83"/>
+      <c r="R10" s="66"/>
+      <c r="S10" s="8">
+        <f t="shared" si="3"/>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="T10" s="57">
+        <v>182</v>
+      </c>
+      <c r="U10" s="75"/>
+      <c r="V10" s="60"/>
+      <c r="W10" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="76"/>
-      <c r="R10" s="81"/>
-      <c r="S10" s="79"/>
-      <c r="T10" s="9">
+        <v>1.8199999999999997E-2</v>
+      </c>
+      <c r="X10" s="51">
+        <v>219</v>
+      </c>
+      <c r="Y10" s="79"/>
+      <c r="Z10" s="54"/>
+      <c r="AA10" s="81">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U10" s="69"/>
-      <c r="V10" s="74"/>
-      <c r="W10" s="72"/>
-      <c r="X10" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.1899999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:27" x14ac:dyDescent="0.3">
       <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="3">
+        <v>4</v>
+      </c>
+      <c r="G11" s="3">
         <v>24</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3">
+        <v>80</v>
+      </c>
+      <c r="I11" s="3">
+        <v>24</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="3">
-        <v>0.44</v>
-      </c>
-      <c r="I11" s="89"/>
-      <c r="J11" s="94"/>
-      <c r="K11" s="92"/>
-      <c r="L11" s="7">
+      <c r="K11" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="L11" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="86"/>
+      <c r="N11" s="72"/>
+      <c r="O11" s="7" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="83"/>
-      <c r="N11" s="95"/>
-      <c r="O11" s="86"/>
-      <c r="P11" s="8">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P11" s="63">
+        <v>228</v>
+      </c>
+      <c r="Q11" s="83"/>
+      <c r="R11" s="66"/>
+      <c r="S11" s="8">
+        <f t="shared" si="3"/>
+        <v>1.4566666666666669E-2</v>
+      </c>
+      <c r="T11" s="57">
+        <v>287</v>
+      </c>
+      <c r="U11" s="75"/>
+      <c r="V11" s="60"/>
+      <c r="W11" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="76"/>
-      <c r="R11" s="81"/>
-      <c r="S11" s="79"/>
-      <c r="T11" s="9">
+        <v>1.8336111111111112E-2</v>
+      </c>
+      <c r="X11" s="51">
+        <v>647</v>
+      </c>
+      <c r="Y11" s="79"/>
+      <c r="Z11" s="54"/>
+      <c r="AA11" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U11" s="69"/>
-      <c r="V11" s="74"/>
-      <c r="W11" s="72"/>
-      <c r="X11" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.1336111111111115E-2</v>
       </c>
     </row>
-    <row r="12" spans="5:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="5:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="4">
+        <v>4</v>
+      </c>
+      <c r="G12" s="4">
+        <v>17</v>
+      </c>
+      <c r="H12" s="4">
+        <v>100</v>
+      </c>
+      <c r="I12" s="4">
         <v>16</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="J12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="4">
-        <v>0.19</v>
-      </c>
-      <c r="I12" s="90"/>
-      <c r="J12" s="100"/>
-      <c r="K12" s="93"/>
-      <c r="L12" s="27">
+      <c r="K12" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="L12" s="70" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" s="87"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="27" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="84"/>
-      <c r="N12" s="101"/>
-      <c r="O12" s="87"/>
-      <c r="P12" s="28">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P12" s="64">
+        <v>307</v>
+      </c>
+      <c r="Q12" s="84"/>
+      <c r="R12" s="67"/>
+      <c r="S12" s="28">
+        <f t="shared" si="3"/>
+        <v>1.5349999999999999E-2</v>
+      </c>
+      <c r="T12" s="58">
+        <v>309</v>
+      </c>
+      <c r="U12" s="76"/>
+      <c r="V12" s="61"/>
+      <c r="W12" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="77"/>
-      <c r="R12" s="102"/>
-      <c r="S12" s="80"/>
-      <c r="T12" s="29">
+        <v>1.5449999999999998E-2</v>
+      </c>
+      <c r="X12" s="52">
+        <v>404</v>
+      </c>
+      <c r="Y12" s="80"/>
+      <c r="Z12" s="55"/>
+      <c r="AA12" s="30">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U12" s="70"/>
-      <c r="V12" s="103"/>
-      <c r="W12" s="73"/>
-      <c r="X12" s="30">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.0199999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="5:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="5:24" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E15" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="34"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
+    <row r="14" spans="5:27" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="5:27" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E15" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="91"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="91"/>
+      <c r="K15" s="91"/>
+      <c r="L15" s="92"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
     </row>
-    <row r="16" spans="5:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="35" t="s">
+    <row r="16" spans="5:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="37"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="96"/>
+      <c r="J16" s="96"/>
+      <c r="K16" s="96"/>
+      <c r="L16" s="97"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
     </row>
-    <row r="17" spans="5:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="38"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="40"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
+    <row r="17" spans="5:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="98"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="93"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="93"/>
+      <c r="J17" s="93"/>
+      <c r="K17" s="93"/>
+      <c r="L17" s="99"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
     </row>
-    <row r="18" spans="5:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="43"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
+    <row r="18" spans="5:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="98" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="93"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="93"/>
+      <c r="K18" s="93"/>
+      <c r="L18" s="99"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
     </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E19" s="38"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="40"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
+    <row r="19" spans="5:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="98"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="93"/>
+      <c r="J19" s="93"/>
+      <c r="K19" s="93"/>
+      <c r="L19" s="99"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
     </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E20" s="44" t="s">
+    <row r="20" spans="5:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="98" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="93"/>
+      <c r="J20" s="93"/>
+      <c r="K20" s="93"/>
+      <c r="L20" s="99"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+    </row>
+    <row r="21" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E21" s="98"/>
+      <c r="F21" s="93"/>
+      <c r="G21" s="93"/>
+      <c r="H21" s="93"/>
+      <c r="I21" s="93"/>
+      <c r="J21" s="93"/>
+      <c r="K21" s="93"/>
+      <c r="L21" s="99"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+    </row>
+    <row r="22" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E22" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="46"/>
+      <c r="F22" s="94"/>
+      <c r="G22" s="94"/>
+      <c r="H22" s="94"/>
+      <c r="I22" s="94"/>
+      <c r="J22" s="94"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="101"/>
     </row>
-    <row r="21" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E21" s="47"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="49"/>
+    <row r="23" spans="5:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="102"/>
+      <c r="F23" s="103"/>
+      <c r="G23" s="103"/>
+      <c r="H23" s="103"/>
+      <c r="I23" s="103"/>
+      <c r="J23" s="103"/>
+      <c r="K23" s="103"/>
+      <c r="L23" s="104"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="U4:X4"/>
-    <mergeCell ref="M3:X3"/>
-    <mergeCell ref="K6:K12"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="W6:W12"/>
-    <mergeCell ref="S6:S12"/>
-    <mergeCell ref="O6:O12"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E16:I17"/>
-    <mergeCell ref="E18:I19"/>
-    <mergeCell ref="E20:I21"/>
+  <mergeCells count="19">
+    <mergeCell ref="X4:AA4"/>
+    <mergeCell ref="P3:AA3"/>
+    <mergeCell ref="U6:U12"/>
+    <mergeCell ref="Y6:Y12"/>
+    <mergeCell ref="Q6:Q12"/>
+    <mergeCell ref="N6:N12"/>
+    <mergeCell ref="T4:W4"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="M6:M12"/>
+    <mergeCell ref="Z6:Z12"/>
+    <mergeCell ref="V6:V12"/>
+    <mergeCell ref="R6:R12"/>
+    <mergeCell ref="E15:L15"/>
+    <mergeCell ref="E16:L17"/>
+    <mergeCell ref="E22:L23"/>
+    <mergeCell ref="E18:L19"/>
+    <mergeCell ref="E20:L21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>